<commit_message>
Added the non vuln files
</commit_message>
<xml_diff>
--- a/Results combined.xlsx
+++ b/Results combined.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Documents/repos/SOEN 691 Static tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C50D9B-C1A1-C644-904D-F1D9D8DF48B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF54E3F4-EB34-DC43-9275-429112483208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet4" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="81">
   <si>
     <t>file_id</t>
   </si>
@@ -223,13 +225,55 @@
   </si>
   <si>
     <t>CWE-79</t>
+  </si>
+  <si>
+    <t>cwe</t>
+  </si>
+  <si>
+    <t>File_id</t>
+  </si>
+  <si>
+    <t>cwe_id</t>
+  </si>
+  <si>
+    <t>models.py</t>
+  </si>
+  <si>
+    <t>methods_upload_user_stats.py</t>
+  </si>
+  <si>
+    <t>metadata.py</t>
+  </si>
+  <si>
+    <t>database.py</t>
+  </si>
+  <si>
+    <t>networking.py</t>
+  </si>
+  <si>
+    <t>rtxcomplete.py</t>
+  </si>
+  <si>
+    <t>views.py</t>
+  </si>
+  <si>
+    <t>playbook.py</t>
+  </si>
+  <si>
+    <t>fckdialog.py</t>
+  </si>
+  <si>
+    <t>routes_general.py</t>
+  </si>
+  <si>
+    <t>server.py</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="8">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -278,8 +322,47 @@
       <color rgb="FF000000"/>
       <name val="&quot;Helvetica Neue&quot;"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;Helvetica Neue&quot;"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -298,8 +381,14 @@
         <bgColor rgb="FFB0B3B2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -367,11 +456,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -409,11 +526,87 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Helvetica Neue"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -441,9 +634,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Sheet2-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="secondRowStripe" dxfId="0"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="firstRowStripe" dxfId="4"/>
+      <tableStyleElement type="secondRowStripe" dxfId="3"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -458,16 +651,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F79">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="file_id"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="filename"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="cve_id"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="cwe_id"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ground truth"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="semgrep"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="bandit"/>
   </tableColumns>
   <tableStyleInfo name="Sheet2-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9FF4269F-5A7E-124C-9C94-41F56DFBC16C}" name="Table2" displayName="Table2" ref="B1:C14" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B1:C14" xr:uid="{9FF4269F-5A7E-124C-9C94-41F56DFBC16C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C14">
+    <sortCondition ref="B1:B14"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{F3B8D598-6B87-624A-8837-ACA5CC9B84EB}" name="filename" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{C2F3B58C-B12E-AA40-80F5-E5BEA5D15C03}" name="cwe" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="Sheet2-style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -672,11 +879,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -694,7 +901,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -1657,24 +1864,344 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="13">
-      <c r="A59" s="4">
+      <c r="A59" s="16">
         <v>360</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D59" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
+      <c r="D59" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+    </row>
+    <row r="60" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A60" s="16">
+        <v>8026</v>
+      </c>
+      <c r="B60" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D60" s="19"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A61" s="16">
+        <v>312</v>
+      </c>
+      <c r="B61" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C61" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D61" s="19"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A62" s="21">
+        <v>8884</v>
+      </c>
+      <c r="B62" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D62" s="19"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A63" s="21">
+        <v>1043</v>
+      </c>
+      <c r="B63" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A64" s="21">
+        <v>403</v>
+      </c>
+      <c r="B64" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C64" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D64" s="19"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A65" s="21">
+        <v>8815</v>
+      </c>
+      <c r="B65" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C65" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D65" s="19"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A66" s="21">
+        <v>8630</v>
+      </c>
+      <c r="B66" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A67" s="22">
+        <v>179</v>
+      </c>
+      <c r="B67" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C67" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D67" s="23"/>
+      <c r="E67" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F67" s="23"/>
+    </row>
+    <row r="68" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A68" s="22">
+        <v>219</v>
+      </c>
+      <c r="B68" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C68" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D68" s="23"/>
+      <c r="E68" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F68" s="23"/>
+    </row>
+    <row r="69" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A69" s="22">
+        <v>261</v>
+      </c>
+      <c r="B69" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C69" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D69" s="23"/>
+      <c r="E69" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F69" s="23"/>
+    </row>
+    <row r="70" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A70" s="22">
+        <v>357</v>
+      </c>
+      <c r="B70" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C70" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D70" s="23"/>
+      <c r="E70" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F70" s="23"/>
+    </row>
+    <row r="71" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A71" s="22">
+        <v>4626</v>
+      </c>
+      <c r="B71" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C71" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D71" s="23"/>
+      <c r="E71" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F71" s="23"/>
+    </row>
+    <row r="72" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A72" s="22">
+        <v>481</v>
+      </c>
+      <c r="B72" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C72" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D72" s="23"/>
+      <c r="E72" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F72" s="23"/>
+    </row>
+    <row r="73" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A73" s="22">
+        <v>7504</v>
+      </c>
+      <c r="B73" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C73" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D73" s="23"/>
+      <c r="E73" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F73" s="23"/>
+    </row>
+    <row r="74" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A74" s="22">
+        <v>8469</v>
+      </c>
+      <c r="B74" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C74" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D74" s="23"/>
+      <c r="E74" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F74" s="23"/>
+    </row>
+    <row r="75" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A75" s="22">
+        <v>8799</v>
+      </c>
+      <c r="B75" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C75" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D75" s="23"/>
+      <c r="E75" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F75" s="23"/>
+    </row>
+    <row r="76" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A76" s="22">
+        <v>8815</v>
+      </c>
+      <c r="B76" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C76" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D76" s="23"/>
+      <c r="E76" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F76" s="23"/>
+    </row>
+    <row r="77" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A77" s="22">
+        <v>8834</v>
+      </c>
+      <c r="B77" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C77" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D77" s="23"/>
+      <c r="E77" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F77" s="23"/>
+    </row>
+    <row r="78" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A78" s="22">
+        <v>8883</v>
+      </c>
+      <c r="B78" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C78" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D78" s="23"/>
+      <c r="E78" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F78" s="23"/>
+    </row>
+    <row r="79" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A79" s="22">
+        <v>8904</v>
+      </c>
+      <c r="B79" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C79" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D79" s="23"/>
+      <c r="E79" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F79" s="23"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A59" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A60 A62:A66" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>AND(ISNUMBER(A2),(NOT(OR(NOT(ISERROR(DATEVALUE(A2))), AND(ISNUMBER(A2), LEFT(CELL("format", A2))="D")))))</formula1>
     </dataValidation>
   </dataValidations>
@@ -1698,6 +2225,205 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394C5430-F896-F949-BA03-A48E5728ADE4}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>179</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>219</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>261</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>357</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>4626</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>481</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7504</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8469</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>8799</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>8815</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>8834</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>8883</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>8904</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA77660E-19E1-AE4A-8599-EFB988CB314A}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" width="36.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2082,7 +2808,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>